<commit_message>
minor updates weapons table
</commit_message>
<xml_diff>
--- a/Game Design/Weapons.xlsx
+++ b/Game Design/Weapons.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Blunt</t>
   </si>
   <si>
-    <t>Fur Coat</t>
-  </si>
-  <si>
     <t>Body Armor</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Critical Block</t>
   </si>
   <si>
-    <t>behavior</t>
-  </si>
-  <si>
     <t>strategic map</t>
   </si>
   <si>
@@ -191,6 +185,15 @@
   </si>
   <si>
     <t>cost 3 AP</t>
+  </si>
+  <si>
+    <t>Fur Coat/Skirt</t>
+  </si>
+  <si>
+    <t>behavior (AI)</t>
+  </si>
+  <si>
+    <t>Husbandry Resistance(for animals)</t>
   </si>
 </sst>
 </file>
@@ -363,21 +366,9 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -385,26 +376,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -420,6 +393,36 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D15:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -771,219 +774,219 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="9"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1003,7 +1006,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1014,197 +1017,197 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="7"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="7"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="9"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="8"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="8" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="8" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="11" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="8"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1230,87 +1233,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="14"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="8"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="7" spans="1:4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1326,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1339,468 +1342,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="21"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="21"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="21"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="21"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="21"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="9"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="9"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="9"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="8"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="16" spans="1:6">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="13" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="12">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="21"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="F19" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="12">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="5"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="12">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="5"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="12">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="5"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="12">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="5"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="24"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="21"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="21"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="22">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="21"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="22">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="21"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="22">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="21"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="22">
+      <c r="E26" s="1"/>
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="16">
         <v>0</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="9"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="22">
-        <v>10</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="9"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="22">
-        <v>10</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="24"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="9"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="22">
-        <v>6</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="9"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="24"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="9"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="26">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="24"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="25"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="31" spans="1:6">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="13" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="12">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="12">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="12">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="21"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="F36" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="12">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="24"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="21"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="21"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="22">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="21"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="22">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="24"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="21"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="22">
-        <v>2</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="21"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18" t="s">
+      <c r="F37" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="5"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="22">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="9"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="18" t="s">
+      <c r="D38" s="12">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="5"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D39" s="12">
+        <v>12</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="5"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="12">
         <v>8</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="24"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="9"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="22">
-        <v>12</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="24"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="9"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="18" t="s">
+      <c r="E40" s="1"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="5"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="22">
-        <v>8</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="9"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="18" t="s">
+      <c r="D41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="5"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="9"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="26">
+      <c r="D42" s="16">
         <v>0</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="24"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="25"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added management documents and minor changes in vision document
</commit_message>
<xml_diff>
--- a/Game Design/Weapons.xlsx
+++ b/Game Design/Weapons.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="23300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,11 @@
     <sheet name="Opponents" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -200,13 +205,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -429,7 +438,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -760,17 +769,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D15:D26"/>
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -861,7 +870,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+    <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -869,7 +878,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="14" spans="1:4" ht="15" thickBot="1"/>
     <row r="15" spans="1:4">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
@@ -980,7 +989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
+    <row r="26" spans="1:4" ht="15" thickBot="1">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -995,25 +1004,30 @@
     <mergeCell ref="A1:B9"/>
     <mergeCell ref="A15:B23"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1078,7 +1092,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+    <row r="9" spans="1:4" ht="15" thickBot="1">
       <c r="A9" s="19"/>
       <c r="B9" s="20"/>
       <c r="C9" s="7" t="s">
@@ -1098,13 +1112,13 @@
       <c r="C11" s="1"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+    <row r="12" spans="1:4" ht="15" thickBot="1">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="14" spans="1:4" ht="15" thickBot="1"/>
     <row r="15" spans="1:4">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
@@ -1181,7 +1195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1">
+    <row r="23" spans="1:4" ht="15" thickBot="1">
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
       <c r="C23" s="7" t="s">
@@ -1203,7 +1217,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
+    <row r="26" spans="1:4" ht="15" thickBot="1">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1214,22 +1228,27 @@
     <mergeCell ref="A1:B9"/>
     <mergeCell ref="A15:B23"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1262,13 +1281,13 @@
       <c r="C4" s="1"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+    <row r="5" spans="1:4" ht="15" thickBot="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22"/>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="6" spans="1:4" ht="15" thickBot="1"/>
     <row r="7" spans="1:4">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
@@ -1309,7 +1328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+    <row r="11" spans="1:4" ht="15" thickBot="1">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="7"/>
@@ -1320,25 +1339,30 @@
     <mergeCell ref="A1:B5"/>
     <mergeCell ref="A7:B11"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1469,7 +1493,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+    <row r="13" spans="1:6" ht="15" thickBot="1">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1477,7 +1501,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="15" thickBot="1"/>
     <row r="16" spans="1:6">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
@@ -1630,7 +1654,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+    <row r="28" spans="1:6" ht="15" thickBot="1">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1638,7 +1662,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="15"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="30" spans="1:6" ht="15" thickBot="1"/>
     <row r="31" spans="1:6">
       <c r="A31" s="23"/>
       <c r="B31" s="24"/>
@@ -1799,7 +1823,7 @@
       <c r="E42" s="1"/>
       <c r="F42" s="14"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1">
+    <row r="43" spans="1:6" ht="15" thickBot="1">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1813,6 +1837,12 @@
     <mergeCell ref="A16:B22"/>
     <mergeCell ref="A31:B37"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>